<commit_message>
Updating assignment 4 grades
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\Documents\GitHub\Bogot-grades\Roster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465C48DC-1472-470B-86A6-2B2498134AFB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41419D6-0437-4F6A-809E-EE89F78C2F2B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A3D61839-BA07-46E1-8D5A-46A1EFB933EE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>ID</t>
   </si>
@@ -53,6 +53,9 @@
   <si>
     <t>Assignment 3</t>
   </si>
+  <si>
+    <t>Assignment 4</t>
+  </si>
 </sst>
 </file>
 
@@ -61,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +84,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -457,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{820B02A1-2325-4B85-8B01-7177D209DAC7}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -471,9 +480,10 @@
     <col min="4" max="4" width="16.85546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,8 +502,11 @@
       <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -512,8 +525,11 @@
       <c r="F2" s="5">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1020815434</v>
       </c>
@@ -532,8 +548,11 @@
       <c r="F3" s="7">
         <v>26.666666666666668</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>1010125106</v>
       </c>
@@ -552,8 +571,11 @@
       <c r="F4" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>55304317</v>
       </c>
@@ -572,8 +594,11 @@
       <c r="F5" s="7">
         <v>75</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>1002154998</v>
       </c>
@@ -592,8 +617,11 @@
       <c r="F6" s="7">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>1143847125</v>
       </c>
@@ -612,8 +640,11 @@
       <c r="F7" s="7">
         <v>96.666666666666671</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>1020405344</v>
       </c>
@@ -632,8 +663,11 @@
       <c r="F8" s="7">
         <v>88.666666666666671</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>1000220414</v>
       </c>
@@ -652,8 +686,11 @@
       <c r="F9" s="7">
         <v>98.666666666666671</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>1026304205</v>
       </c>
@@ -672,8 +709,11 @@
       <c r="F10" s="7">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>355061</v>
       </c>
@@ -692,8 +732,11 @@
       <c r="F11" s="7">
         <v>94.666666666666671</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>1018508749</v>
       </c>
@@ -712,8 +755,11 @@
       <c r="F12" s="7">
         <v>96.666666666666671</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>70253417</v>
       </c>
@@ -732,8 +778,11 @@
       <c r="F13" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>1136888718</v>
       </c>
@@ -752,8 +801,11 @@
       <c r="F14" s="7">
         <v>98.666666666666671</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>293841098</v>
       </c>
@@ -772,8 +824,11 @@
       <c r="F15" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>1072714383</v>
       </c>
@@ -792,8 +847,11 @@
       <c r="F16" s="7">
         <v>98.666666666666671</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>1010243078</v>
       </c>
@@ -812,8 +870,11 @@
       <c r="F17" s="7">
         <v>98.666666666666671</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" s="3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>1007351402</v>
       </c>
@@ -832,8 +893,11 @@
       <c r="F18" s="7">
         <v>98.666666666666671</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>1002996359</v>
       </c>
@@ -852,8 +916,11 @@
       <c r="F19" s="7">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>1010236320</v>
       </c>
@@ -872,8 +939,11 @@
       <c r="F20" s="7">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>1020845574</v>
       </c>
@@ -892,8 +962,11 @@
       <c r="F21" s="7">
         <v>100</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>1020729394</v>
       </c>
@@ -907,13 +980,16 @@
         <v>100</v>
       </c>
       <c r="E22" s="7">
-        <v>5.882352941176471</v>
+        <v>88.24</v>
       </c>
       <c r="F22" s="7">
         <v>85.333333333333329</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22" s="3">
+        <v>93.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>80039961</v>
       </c>
@@ -932,8 +1008,11 @@
       <c r="F23" s="7">
         <v>75.999999999999986</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>1026304547</v>
       </c>
@@ -952,8 +1031,11 @@
       <c r="F24" s="7">
         <v>92</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>1088328190</v>
       </c>
@@ -972,8 +1054,11 @@
       <c r="F25" s="7">
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>1072706035</v>
       </c>
@@ -992,8 +1077,11 @@
       <c r="F26" s="7">
         <v>100</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>1032453588</v>
       </c>
@@ -1012,8 +1100,11 @@
       <c r="F27" s="7">
         <v>75.333333333333329</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>1014288458</v>
       </c>
@@ -1032,8 +1123,11 @@
       <c r="F28" s="7">
         <v>100</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>1143877513</v>
       </c>
@@ -1052,8 +1146,11 @@
       <c r="F29" s="7">
         <v>100</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>1019131372</v>
       </c>
@@ -1072,8 +1169,11 @@
       <c r="F30" s="7">
         <v>95.999999999999986</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>1136880643</v>
       </c>
@@ -1092,8 +1192,11 @@
       <c r="F31" s="7">
         <v>100</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>1018508173</v>
       </c>
@@ -1112,8 +1215,11 @@
       <c r="F32" s="7">
         <v>78</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>1004133287</v>
       </c>
@@ -1132,8 +1238,11 @@
       <c r="F33" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>1015468827</v>
       </c>
@@ -1152,8 +1261,11 @@
       <c r="F34" s="7">
         <v>100</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>1143372208</v>
       </c>
@@ -1172,8 +1284,11 @@
       <c r="F35" s="7">
         <v>100</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>1014264765</v>
       </c>
@@ -1192,8 +1307,11 @@
       <c r="F36" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G36" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>1018503227</v>
       </c>
@@ -1212,8 +1330,11 @@
       <c r="F37" s="7">
         <v>100</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>1015448479</v>
       </c>
@@ -1232,8 +1353,11 @@
       <c r="F38" s="7">
         <v>98.666666666666671</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G38" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>1018496783</v>
       </c>
@@ -1252,8 +1376,11 @@
       <c r="F39" s="7">
         <v>82</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>1071171655</v>
       </c>
@@ -1272,8 +1399,11 @@
       <c r="F40" s="7">
         <v>100</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G40" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>1020821245</v>
       </c>
@@ -1292,8 +1422,11 @@
       <c r="F41" s="7">
         <v>100</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G41" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>80774647</v>
       </c>
@@ -1312,8 +1445,11 @@
       <c r="F42" s="7">
         <v>95.333333333333329</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G42" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>1056076234</v>
       </c>
@@ -1332,8 +1468,12 @@
       <c r="F43" s="7">
         <v>0</v>
       </c>
+      <c r="G43" s="3">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>